<commit_message>
working GUI.py + object avoidance
</commit_message>
<xml_diff>
--- a/Laptop setup/GUI/ImagesSheet.xlsx
+++ b/Laptop setup/GUI/ImagesSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7360" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reading" sheetId="1" state="visible" r:id="rId1"/>
@@ -338,10 +338,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C34"/>
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -369,7 +369,7 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="n"/>
       <c r="E2" s="1" t="n"/>
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="n"/>
       <c r="E3" s="1" t="n"/>
@@ -393,7 +393,7 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="n"/>
       <c r="E4" s="1" t="n"/>
@@ -405,42 +405,157 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="n"/>
       <c r="E5" s="1" t="n"/>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="3">
-      <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="n"/>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>w3</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="D6" s="1" t="n"/>
       <c r="E6" s="1" t="n"/>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="3">
-      <c r="A7" s="1" t="n"/>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>w3</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
       <c r="D7" s="1" t="n"/>
       <c r="E7" s="1" t="n"/>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="3">
-      <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="n"/>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>w4</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="D8" s="1" t="n"/>
       <c r="E8" s="1" t="n"/>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="3">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1" s="3"/>
-    <row r="11" ht="15.75" customHeight="1" s="3"/>
-    <row r="12" ht="15.75" customHeight="1" s="3"/>
-    <row r="13" ht="15.75" customHeight="1" s="3"/>
-    <row r="14" ht="15.75" customHeight="1" s="3"/>
-    <row r="15" ht="15.75" customHeight="1" s="3"/>
-    <row r="16" ht="15.75" customHeight="1" s="3"/>
-    <row r="17" ht="15.75" customHeight="1" s="3"/>
-    <row r="18" ht="15.75" customHeight="1" s="3"/>
-    <row r="19" ht="15.75" customHeight="1" s="3"/>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>w4</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" s="3">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>w5</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1" s="3">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>w5</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" s="3">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>w6</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" s="3">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>w6</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" s="3">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>w7</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" s="3">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>w7</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1" s="3">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>w8</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1" s="3">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>w8</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1" s="3">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>w9</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1" s="3">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>w9</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2</v>
+      </c>
+    </row>
     <row r="20" ht="15.75" customHeight="1" s="3"/>
     <row r="21" ht="15.75" customHeight="1" s="3"/>
     <row r="22" ht="15.75" customHeight="1" s="3"/>

</xml_diff>

<commit_message>
run GUI from, pyqt6 -> pyqt5
</commit_message>
<xml_diff>
--- a/Laptop setup/GUI/ImagesSheet.xlsx
+++ b/Laptop setup/GUI/ImagesSheet.xlsx
@@ -369,7 +369,7 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>2</v>
+        <v/>
       </c>
       <c r="D2" s="1" t="n"/>
       <c r="E2" s="1" t="n"/>
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>2</v>
+        <v/>
       </c>
       <c r="D3" s="1" t="n"/>
       <c r="E3" s="1" t="n"/>
@@ -393,7 +393,7 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>2</v>
+        <v/>
       </c>
       <c r="D4" s="1" t="n"/>
       <c r="E4" s="1" t="n"/>
@@ -405,7 +405,7 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>2</v>
+        <v/>
       </c>
       <c r="D5" s="1" t="n"/>
       <c r="E5" s="1" t="n"/>
@@ -417,7 +417,7 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>2</v>
+        <v/>
       </c>
       <c r="D6" s="1" t="n"/>
       <c r="E6" s="1" t="n"/>
@@ -429,7 +429,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v/>
       </c>
       <c r="D7" s="1" t="n"/>
       <c r="E7" s="1" t="n"/>
@@ -441,7 +441,7 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>2</v>
+        <v/>
       </c>
       <c r="D8" s="1" t="n"/>
       <c r="E8" s="1" t="n"/>
@@ -453,7 +453,7 @@
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="3">
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="3">
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="3">
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="3">
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="3">
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="3">
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="3">
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="3">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="3">
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="3">
@@ -553,7 +553,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="3"/>

</xml_diff>